<commit_message>
Update Scrum Status Forms w Task List 2025,04,08.xlsx
</commit_message>
<xml_diff>
--- a/ByteJumper/ByteJumper/Scrum/Scrum Status Forms w Task List 2025,04,08.xlsx
+++ b/ByteJumper/ByteJumper/Scrum/Scrum Status Forms w Task List 2025,04,08.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Visual Studio 2022\CSC2025\MyCode\ByteJumper\AssemblyFinal\ByteJumper\ByteJumper\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93C8EB99-0B86-4AC9-85CD-88E3B8BFF3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F198A25-31EA-4324-89BB-4D978FB12BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-5145" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="72">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -229,6 +229,33 @@
   </si>
   <si>
     <t>Debugging</t>
+  </si>
+  <si>
+    <t>Ethan Eye Aaron Villalobos</t>
+  </si>
+  <si>
+    <t>Start Screen</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>PlayerMovement</t>
+  </si>
+  <si>
+    <t>Develop procedure to display start screen</t>
+  </si>
+  <si>
+    <t>Develop procedure to display player with ascii char</t>
+  </si>
+  <si>
+    <t>Set up procedure to display obstacles</t>
+  </si>
+  <si>
+    <t>Set up procedure to have player move according to input made by user</t>
   </si>
 </sst>
 </file>
@@ -371,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,6 +454,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -901,24 +931,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4BDE91-026E-42C1-9643-D39E9BFB7C68}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:C49"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.41015625" customWidth="1"/>
-    <col min="3" max="3" width="66.87890625" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="66.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -926,7 +956,7 @@
         <v>45757</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -935,7 +965,7 @@
         <v>45762</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -943,7 +973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -951,7 +981,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -959,13 +989,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -973,29 +1003,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -1004,7 +1034,7 @@
         <v>45762</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1026,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -1037,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -1048,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>56</v>
       </c>
@@ -1059,7 +1089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>52</v>
       </c>
@@ -1070,7 +1100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>52</v>
       </c>
@@ -1081,7 +1111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>56</v>
       </c>
@@ -1092,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>55</v>
       </c>
@@ -1103,7 +1133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>55</v>
       </c>
@@ -1114,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>55</v>
       </c>
@@ -1125,7 +1155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>56</v>
       </c>
@@ -1136,72 +1166,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:4" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="12"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C31" s="13"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C32" s="13"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" s="13"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" s="13"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" s="13"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" s="13"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" s="13"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" s="13"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" s="13"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" s="13"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" s="13"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" s="13"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" s="13"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" s="13"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" s="13"/>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" s="13"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.5">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" s="13"/>
     </row>
-    <row r="49" spans="3:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C49" s="14"/>
     </row>
   </sheetData>
@@ -1220,19 +1250,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1266,7 +1296,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1275,37 +1305,37 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1313,7 +1343,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1325,7 +1387,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1333,52 +1395,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B18" t="str">
-        <f>Cover!B18</f>
-        <v>All</v>
-      </c>
-      <c r="C18" t="str">
-        <f>Cover!C18</f>
-        <v>Decide on Project</v>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
       </c>
       <c r="D18" s="1">
         <f>Cover!D18</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B19" t="str">
-        <f>Cover!B19</f>
-        <v>All</v>
-      </c>
-      <c r="C19" t="str">
-        <f>Cover!C19</f>
-        <v>Identify major parts of the project</v>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
       </c>
       <c r="D19" s="1">
-        <f>Cover!D19</f>
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B20" t="str">
-        <f>Cover!B20</f>
-        <v>All</v>
-      </c>
-      <c r="C20" t="str">
-        <f>Cover!C20</f>
-        <v>Set up GitHub account and invite all participants including WayneWCook</v>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
       </c>
       <c r="D20" s="1">
-        <f>Cover!D20</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="D21" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1387,7 +1449,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1395,7 +1457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>24</v>
       </c>
@@ -1406,7 +1468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -1417,7 +1479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>28</v>
       </c>
@@ -1434,6 +1496,7 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1445,15 +1508,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1466,7 +1529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1487,7 +1550,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1496,7 +1559,7 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1504,7 +1567,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1512,7 +1575,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1520,13 +1583,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1534,7 +1597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1546,7 +1609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1554,7 +1617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f>'15 Apr'!B31</f>
         <v>All</v>
@@ -1568,7 +1631,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f>'15 Apr'!B32</f>
         <v>TBA</v>
@@ -1582,7 +1645,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f>'15 Apr'!B33</f>
         <v>TBA</v>
@@ -1596,7 +1659,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1605,7 +1668,7 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1613,7 +1676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>28</v>
       </c>
@@ -1624,7 +1687,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -1635,7 +1698,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>28</v>
       </c>
@@ -1663,15 +1726,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +1747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1705,7 +1768,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1714,7 +1777,7 @@
         <v>45772</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1722,7 +1785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1730,7 +1793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1738,13 +1801,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="16"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1752,7 +1815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1764,7 +1827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1772,7 +1835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="str">
         <f>'18 Apr'!B31</f>
         <v>TBA</v>
@@ -1786,7 +1849,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" t="str">
         <f>'18 Apr'!B32</f>
         <v>TBA</v>
@@ -1800,7 +1863,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" t="str">
         <f>'18 Apr'!B33</f>
         <v>TBA</v>
@@ -1814,7 +1877,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1823,7 +1886,7 @@
         <v>45772</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1848,15 +1911,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1869,7 +1932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1890,7 +1953,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1899,7 +1962,7 @@
         <v>45783</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1907,7 +1970,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1915,7 +1978,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1923,13 +1986,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="16"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1937,7 +2000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1949,7 +2012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1957,7 +2020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1966,7 +2029,7 @@
         <v>45783</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1991,15 +2054,15 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2033,7 +2096,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2042,7 +2105,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2050,7 +2113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2058,7 +2121,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2066,13 +2129,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="16"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2080,7 +2143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2092,7 +2155,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2100,7 +2163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2109,7 +2172,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2117,7 +2180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>41</v>
       </c>
@@ -2128,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>43</v>
       </c>
@@ -2139,7 +2202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>44</v>
       </c>
@@ -2150,7 +2213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>42</v>
       </c>
@@ -2178,15 +2241,15 @@
       <selection activeCell="B10" sqref="B10:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.35" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2210,7 +2273,7 @@
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -2233,7 +2296,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2242,7 +2305,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2259,7 +2322,7 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2276,7 +2339,7 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2293,7 +2356,7 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -2304,7 +2367,7 @@
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
@@ -2319,7 +2382,7 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2336,7 +2399,7 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" t="str">
         <f>'6 May'!B31</f>
         <v>Video</v>
@@ -2359,7 +2422,7 @@
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" t="str">
         <f>'6 May'!B32</f>
         <v>Slides</v>
@@ -2382,7 +2445,7 @@
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" t="str">
         <f>'6 May'!B33</f>
         <v>Presentation</v>
@@ -2405,7 +2468,7 @@
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" t="str">
         <f>'6 May'!B34</f>
         <v>Project</v>
@@ -2428,7 +2491,7 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -2439,7 +2502,7 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -2450,7 +2513,7 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2468,7 +2531,7 @@
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2488,7 +2551,7 @@
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>36</v>
       </c>
@@ -2505,7 +2568,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>37</v>
       </c>
@@ -2522,7 +2585,7 @@
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>38</v>
       </c>
@@ -2539,7 +2602,7 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>39</v>
       </c>
@@ -2556,7 +2619,7 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -2567,7 +2630,7 @@
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -2578,7 +2641,7 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -2589,7 +2652,7 @@
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -2600,7 +2663,7 @@
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -2611,7 +2674,7 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -2622,7 +2685,7 @@
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -2633,7 +2696,7 @@
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2651,7 +2714,7 @@
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2668,7 +2731,7 @@
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>23</v>
       </c>
@@ -2682,7 +2745,7 @@
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -2693,7 +2756,7 @@
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
     </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.5">
+    <row r="33" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
@@ -2704,7 +2767,7 @@
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.5">
+    <row r="34" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -2715,7 +2778,7 @@
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
     </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.5">
+    <row r="35" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -2739,6 +2802,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE5E75FC1DF6F145BFAEC137222EE7DF" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cec7c1021bc7ce9566b3d60a148821a1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3c090fe0-0a85-46c2-a6a0-5610b56c0757" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c95b3c89d5ab0ef8111e8a7a83c6b8a1" ns2:_="">
     <xsd:import namespace="3c090fe0-0a85-46c2-a6a0-5610b56c0757"/>
@@ -2876,35 +2954,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15BDA74C-906D-4E42-BAAC-8AC16CF01DA0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9347D2B2-E22F-48F2-891B-DE352B9216F7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3c090fe0-0a85-46c2-a6a0-5610b56c0757"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2926,9 +2979,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9347D2B2-E22F-48F2-891B-DE352B9216F7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15BDA74C-906D-4E42-BAAC-8AC16CF01DA0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3c090fe0-0a85-46c2-a6a0-5610b56c0757"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>